<commit_message>
NIH Terminations Data Analysis Final 5.18.25
</commit_message>
<xml_diff>
--- a/NIH Terminated Grants Pitch/Grant Percent Termination by Grant Family.xlsx
+++ b/NIH Terminated Grants Pitch/Grant Percent Termination by Grant Family.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neelajain/dataProjects/NIH Terminated Grants Pitch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neelajain/dataProjects/2025-NIH-NYC-Funding/NIH Terminated Grants Pitch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F87DF81B-ADC0-C349-B600-269B107B9E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4456F35E-E4F0-4344-B35F-0F4E1C935E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="1040" windowWidth="28040" windowHeight="17440" xr2:uid="{678BC1E8-66BF-F04B-943F-3FE2F9A212C9}"/>
   </bookViews>
   <sheets>
     <sheet name="terminated_grants" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -971,7 +972,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,19 +1001,22 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>403</v>
+      </c>
+      <c r="C2">
+        <v>52698</v>
+      </c>
+      <c r="D2">
         <f>B2+C2</f>
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
+        <v>53101</v>
+      </c>
+      <c r="E2">
         <f>(B2/D2)*100</f>
-        <v>100</v>
+        <v>0.7589310935763921</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -1020,40 +1024,40 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>5799</v>
       </c>
       <c r="D3">
         <f>B3+C3</f>
-        <v>53</v>
+        <v>5897</v>
       </c>
       <c r="E3">
         <f>(B3/D3)*100</f>
-        <v>5.6603773584905666</v>
+        <v>1.6618619637103611</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C4">
-        <v>408</v>
+        <v>5212</v>
       </c>
       <c r="D4">
         <f>B4+C4</f>
-        <v>419</v>
+        <v>5246</v>
       </c>
       <c r="E4">
         <f>(B4/D4)*100</f>
-        <v>2.6252983293556085</v>
+        <v>0.64811284788410217</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1077,141 +1081,151 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>323</v>
+        <v>2070</v>
       </c>
       <c r="D6">
         <f>B6+C6</f>
-        <v>329</v>
+        <v>2100</v>
       </c>
       <c r="E6">
         <f>(B6/D6)*100</f>
-        <v>1.8237082066869299</v>
+        <v>1.4285714285714286</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>5799</v>
+        <v>1442</v>
       </c>
       <c r="D7">
         <f>B7+C7</f>
-        <v>5897</v>
+        <v>1463</v>
       </c>
       <c r="E7">
         <f>(B7/D7)*100</f>
-        <v>1.6618619637103611</v>
+        <v>1.4354066985645932</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>1442</v>
+        <v>801</v>
       </c>
       <c r="D8">
         <f>B8+C8</f>
-        <v>1463</v>
+        <v>810</v>
       </c>
       <c r="E8">
         <f>(B8/D8)*100</f>
-        <v>1.4354066985645932</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>2070</v>
+        <v>408</v>
       </c>
       <c r="D9">
         <f>B9+C9</f>
-        <v>2100</v>
+        <v>419</v>
       </c>
       <c r="E9">
         <f>(B9/D9)*100</f>
-        <v>1.4285714285714286</v>
+        <v>2.6252983293556085</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>801</v>
+        <v>323</v>
       </c>
       <c r="D10">
         <f>B10+C10</f>
-        <v>810</v>
+        <v>329</v>
       </c>
       <c r="E10">
         <f>(B10/D10)*100</f>
-        <v>1.1111111111111112</v>
+        <v>1.8237082066869299</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>403</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>52698</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <f>B11+C11</f>
-        <v>53101</v>
+        <v>53</v>
       </c>
       <c r="E11">
         <f>(B11/D11)*100</f>
-        <v>0.7589310935763921</v>
+        <v>5.6603773584905666</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>34</v>
-      </c>
-      <c r="C12">
-        <v>5212</v>
-      </c>
-      <c r="D12">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
         <f>B12+C12</f>
-        <v>5246</v>
-      </c>
-      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
         <f>(B12/D12)*100</f>
-        <v>0.64811284788410217</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
-    <sortCondition descending="1" ref="E1:E15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition descending="1" ref="D1:D13"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5A6279-FFF8-3948-86E6-EEE78D5051DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>